<commit_message>
Figures and Final report
</commit_message>
<xml_diff>
--- a/results/Confusion Matrix.xlsx
+++ b/results/Confusion Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16640" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16640" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -455,7 +455,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -527,6 +527,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -637,7 +665,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="99">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="4" builtinId="34"/>
     <cellStyle name="60% - Accent1" xfId="2" builtinId="32"/>
@@ -676,6 +704,20 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
@@ -708,6 +750,20 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1296,7 +1352,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A17" sqref="A17:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1778,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I19" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -2270,7 +2326,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A11"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -2755,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>

</xml_diff>